<commit_message>
Allow GC's to hide medicare fields
</commit_message>
<xml_diff>
--- a/test/fixtures/files/invalid_mysyg_setting.xlsx
+++ b/test/fixtures/files/invalid_mysyg_setting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t xml:space="preserve">RowID</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">RequireEmerg</t>
   </si>
   <si>
-    <t xml:space="preserve">RequireMedical</t>
+    <t xml:space="preserve">MedicareOption</t>
   </si>
   <si>
     <t xml:space="preserve">ApproveOption</t>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide</t>
   </si>
   <si>
     <t xml:space="preserve">Invalid</t>
@@ -116,6 +119,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -203,11 +207,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.32"/>
@@ -215,17 +219,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.2"/>
   </cols>
   <sheetData>
@@ -341,16 +345,16 @@
         <v>24</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>